<commit_message>
More bibliographic work. Knowledge Map started
</commit_message>
<xml_diff>
--- a/bibliografia/resumen_bibliografia.xlsx
+++ b/bibliografia/resumen_bibliografia.xlsx
@@ -5,28 +5,40 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\José Enrique\Desktop\cell-formation\cell-formation\bibliografia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josee\Desktop\Departamento\formacion celulas\reproduccion_ulutas\bibliografia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C77633D-461C-4D3A-BFB4-71F81BE33D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCF7E3A-E32D-404A-B111-F7DE1A4EB681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1080" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Algorithms" sheetId="1" r:id="rId1"/>
+    <sheet name="Articles" sheetId="1" r:id="rId1"/>
     <sheet name="Reviews" sheetId="2" r:id="rId2"/>
+    <sheet name="ReviewKesavan2019" sheetId="3" r:id="rId3"/>
+    <sheet name="ReviewPapaioannu2010" sheetId="5" r:id="rId4"/>
+    <sheet name="diccionario" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="163">
   <si>
     <t>Autor/res</t>
   </si>
@@ -237,33 +249,18 @@
     <t>Chaudhuri</t>
   </si>
   <si>
-    <t>multi-objective CFP</t>
-  </si>
-  <si>
-    <t>1 cita (de ellos mismos)</t>
-  </si>
-  <si>
     <t>Seema</t>
   </si>
   <si>
     <t>0 CITAS</t>
   </si>
   <si>
-    <t>soft computing techniques for CFP</t>
-  </si>
-  <si>
     <t>Kesavan</t>
   </si>
   <si>
-    <t>heuristic and meta-heuristic algorithms</t>
-  </si>
-  <si>
     <t>Comentarios</t>
   </si>
   <si>
-    <t>2 Citas.</t>
-  </si>
-  <si>
     <t>Karoum</t>
   </si>
   <si>
@@ -285,9 +282,6 @@
     <t>Papaioannou</t>
   </si>
   <si>
-    <t>160ypico citas</t>
-  </si>
-  <si>
     <t>MUY COMPLETO</t>
   </si>
   <si>
@@ -312,59 +306,345 @@
     <t>Yin</t>
   </si>
   <si>
-    <t>Taxonomy and Review</t>
-  </si>
-  <si>
     <t>Delgoshaei</t>
   </si>
   <si>
-    <t>REVIEW CLUSTERING</t>
-  </si>
-  <si>
-    <t>Evolution of clustering techniques in designing cellular manufacturing systems: A state-of-art review</t>
-  </si>
-  <si>
     <r>
-      <t>Similarity coefficient methods applied to the cell</t>
+      <t xml:space="preserve">heuristic and meta-heuristic algorithms in </t>
     </r>
     <r>
       <rPr>
-        <sz val="24"/>
-        <color rgb="FF2E2E2E"/>
-        <rFont val="Georgia"/>
-        <family val="1"/>
-      </rPr>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>formation</t>
+      <t>CMS</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="24"/>
-        <color rgb="FF2E2E2E"/>
-        <rFont val="Georgia"/>
-        <family val="1"/>
-      </rPr>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>problem: A taxonomy and Review</t>
-    </r>
+  </si>
+  <si>
+    <t>Saraç and Ozcelik</t>
+  </si>
+  <si>
+    <t>CF - GE</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>14 problemas, mejoró 8</t>
+  </si>
+  <si>
+    <t>Tuning del GA con diferentes tipos de mutaciones y reproducciones</t>
+  </si>
+  <si>
+    <t>SA, TS, original GA, AS and CNN</t>
+  </si>
+  <si>
+    <t>Husseinzadeh et al</t>
+  </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>GGA</t>
+  </si>
+  <si>
+    <t>40 problemas, mejoró 23</t>
+  </si>
+  <si>
+    <t>Mahmoodian et al.</t>
+  </si>
+  <si>
+    <t>GBPSO (particle swarm)</t>
+  </si>
+  <si>
+    <t>discrete</t>
+  </si>
+  <si>
+    <t>Pachayappan</t>
+  </si>
+  <si>
+    <t>machine-component</t>
+  </si>
+  <si>
+    <t>HGA</t>
+  </si>
+  <si>
+    <t>ZODIAC and GRAFICS</t>
+  </si>
+  <si>
+    <t>ideal seed heuristic</t>
+  </si>
+  <si>
+    <t>James et al.</t>
+  </si>
+  <si>
+    <t>MPCF</t>
+  </si>
+  <si>
+    <t>PSO</t>
+  </si>
+  <si>
+    <t>ZODIAC, GRAFICS, MST, GATSP, GA, GP, EA</t>
+  </si>
+  <si>
+    <t>HGGA</t>
+  </si>
+  <si>
+    <t>*local search
+*rank-based roulette wheel
+*2 point crossover operator with the repair</t>
+  </si>
+  <si>
+    <t>Wu et al.</t>
+  </si>
+  <si>
+    <t>25 problemas, 18 mejoró</t>
+  </si>
+  <si>
+    <t>SA(simulated annealing)</t>
+  </si>
+  <si>
+    <t>IPSO (particle swarm)</t>
+  </si>
+  <si>
+    <t>le añade inteligencia con una red neuronal (SOM)</t>
+  </si>
+  <si>
+    <t>35 problemas, 30 mejoró</t>
+  </si>
+  <si>
+    <t>ZODIAC, TSP-GA, GA</t>
+  </si>
+  <si>
+    <t>Wang et al.</t>
+  </si>
+  <si>
+    <t>dispatching rules for a joint decision of cell formation and parts scheduling in batches</t>
+  </si>
+  <si>
+    <t>CFPSC</t>
+  </si>
+  <si>
+    <t>SSPPO</t>
+  </si>
+  <si>
+    <t>SSSPT, SSODD, SSFIFO</t>
+  </si>
+  <si>
+    <t>Bajestani et al.</t>
+  </si>
+  <si>
+    <t>Solimanpur et al</t>
+  </si>
+  <si>
+    <t>Kamalakannan et al</t>
+  </si>
+  <si>
+    <t>Karoum et al</t>
+  </si>
+  <si>
+    <t>Gómez et al.</t>
+  </si>
+  <si>
+    <t>MILP</t>
+  </si>
+  <si>
+    <t>TS</t>
+  </si>
+  <si>
+    <t>11 problemas, 5 mejoró, 3 igualó</t>
+  </si>
+  <si>
+    <t>TS - multithread processing</t>
+  </si>
+  <si>
+    <t>TS - short term memory and overall iteartive searching</t>
+  </si>
+  <si>
+    <t>ACO</t>
+  </si>
+  <si>
+    <t>MOSS with MADM</t>
+  </si>
+  <si>
+    <t>cell load and cost minimization</t>
+  </si>
+  <si>
+    <t>SPEA-II and NSGA-I</t>
+  </si>
+  <si>
+    <t>ZODIAC, GRAFICS, MST-Clustering, GATSP, GA and EA</t>
+  </si>
+  <si>
+    <t>sequence, production volume, intercellular movements and voids</t>
+  </si>
+  <si>
+    <t>16 problemas, mejoró 5</t>
+  </si>
+  <si>
+    <t>8 problemas, mejoró 4</t>
+  </si>
+  <si>
+    <t>CLASS, clustering, minimun spanning tree, GA, NN</t>
+  </si>
+  <si>
+    <t>ZODIAC, GRAFICS, EA, SA, GRASP, GA and large neighbour search</t>
+  </si>
+  <si>
+    <t>35 problemas, 31 mejoró</t>
+  </si>
+  <si>
+    <t>10 problemas</t>
+  </si>
+  <si>
+    <t>12 problemas</t>
+  </si>
+  <si>
+    <t>HCS - local search</t>
+  </si>
+  <si>
+    <t>SIGLAS</t>
+  </si>
+  <si>
+    <t>NOMBRE DEL MÉTODO</t>
+  </si>
+  <si>
+    <t>Tabu Search</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>Cuckoo Search</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>Particle Swarm</t>
+  </si>
+  <si>
+    <t>Simulated Annealing</t>
+  </si>
+  <si>
+    <t>NOMBRE DEL PROBLEMA</t>
+  </si>
+  <si>
+    <t>CFP</t>
+  </si>
+  <si>
+    <t>Cell Formation Problem</t>
+  </si>
+  <si>
+    <t>Machine-part Cell Formation</t>
+  </si>
+  <si>
+    <t>CSA</t>
+  </si>
+  <si>
+    <t>160+ citas</t>
+  </si>
+  <si>
+    <t>Taxonomy and 
+Review</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>Scatter Search</t>
+  </si>
+  <si>
+    <t>MOCF</t>
+  </si>
+  <si>
+    <t>Multi-objective Cell Formation</t>
+  </si>
+  <si>
+    <t>DCF</t>
+  </si>
+  <si>
+    <t>Dynamic Cell Formation</t>
+  </si>
+  <si>
+    <t>Mixed-integer linear programming</t>
+  </si>
+  <si>
+    <t>CFP and cell-layout</t>
+  </si>
+  <si>
+    <t>soft computing techniques</t>
+  </si>
+  <si>
+    <t>CMS</t>
+  </si>
+  <si>
+    <t>CLUSTERING</t>
+  </si>
+  <si>
+    <t>CMS design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Similarity coefficient methods </t>
+  </si>
+  <si>
+    <t>2 Citas. Cita artículos algo más modernos. Se centra en heurísticas y meta-heurísticas de CFP y Cell-layout. Concluye que para enfrentar multiples problemas del CMS hace falta una hibridación metaheurística robusta. Multi-optimization da peores resultados individuales</t>
+  </si>
+  <si>
+    <t>Mehdizadeh</t>
+  </si>
+  <si>
+    <t>Zohrevand</t>
+  </si>
+  <si>
+    <t>1 cita (de ellos mismos). 2016 es el año más moderno (mehdizadeh y zohrevand)</t>
+  </si>
+  <si>
+    <t>14 citas en Computer and Industrial Engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiobjetivo: </t>
+  </si>
+  <si>
+    <t>Vibration damping optimization</t>
+  </si>
+  <si>
+    <t>Lashgari</t>
+  </si>
+  <si>
+    <t>31 citas en Computer and Industrial Engineering</t>
+  </si>
+  <si>
+    <t>Stochastic programming</t>
+  </si>
+  <si>
+    <t>Multiobjetivo:</t>
+  </si>
+  <si>
+    <t>Robust optimisation to design a dynamic cellular manufacturing system integrating group layout and workers' assignment</t>
+  </si>
+  <si>
+    <t>Li</t>
+  </si>
+  <si>
+    <t>3 citas en Computer and Industrial Engineering</t>
+  </si>
+  <si>
+    <t>A novel algorithm of cell formation with alternative machines and multiple-operation type machines</t>
+  </si>
+  <si>
+    <t>0 citas en European Journal of Industrial Engineering
+NO CONSIGO EL ARTICULO</t>
+  </si>
+  <si>
+    <t>Multi-objective CFP</t>
   </si>
 </sst>
 </file>
@@ -412,22 +692,25 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="24"/>
-      <color rgb="FF2E2E2E"/>
-      <name val="Georgia"/>
-      <family val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -444,7 +727,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -461,11 +744,77 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -485,9 +834,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -506,14 +852,45 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -795,10 +1172,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,29 +1191,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" s="9" t="s">
+      <c r="E1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="9" t="s">
-        <v>43</v>
+      <c r="H1" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -912,261 +1289,187 @@
         <v>11</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="3">
         <v>2020</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>20</v>
+        <v>29</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="3">
         <v>2020</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>29</v>
+      <c r="C7" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="F8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B9" s="3">
         <v>2019</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2" t="s">
-        <v>26</v>
+      <c r="C9" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B10" s="3">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B11" s="3">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="5">
-        <v>2017</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" s="15">
-        <v>2019</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>63</v>
+        <v>51</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2016</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B13" s="3">
+        <v>2016</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="15"/>
+        <v>156</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>153</v>
       </c>
       <c r="B14" s="3">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>44</v>
+        <v>157</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B15" s="3">
+        <v>2021</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1987</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="3">
-        <v>2017</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" s="3">
-        <v>2016</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-    </row>
-    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B24" s="3">
-        <v>2006</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="13">
-        <v>2010</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="3">
-        <v>1987</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1176,6 +1479,537 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE49079E-D804-408A-9E73-9DA75E4351D1}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24" customWidth="1"/>
+    <col min="8" max="8" width="71.85546875" style="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="24">
+        <v>2020</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2017</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2019</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2020</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="12">
+        <v>2019</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="F6" s="12"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="28">
+        <v>2010</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2006</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F8" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FE4DF2F-9F61-475D-818B-C641491726AD}">
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="77.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2012</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2014</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2007</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2008</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="16">
+        <v>2010</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2009</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2010</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2014</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2012</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25C2CA28-7F3F-4E71-8CEB-37F843BC94D3}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1184,4 +2018,271 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F67EBF-2A64-4E23-9654-8BB6149B5AE4}">
+  <dimension ref="A1:E31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="21"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="21"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="21"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" s="20"/>
+      <c r="E8" s="21"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="20"/>
+      <c r="E9" s="21"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="21"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="21"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="20"/>
+      <c r="B13" s="21"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
+      <c r="B14" s="21"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="21"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
+      <c r="B15" s="21"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="20"/>
+      <c r="B16" s="21"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="20"/>
+      <c r="B17" s="21"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="21"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
+      <c r="B18" s="21"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="20"/>
+      <c r="B19" s="21"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="21"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="20"/>
+      <c r="B20" s="21"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="21"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="20"/>
+      <c r="B21" s="21"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="21"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="20"/>
+      <c r="B22" s="21"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="20"/>
+      <c r="B23" s="21"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="21"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="20"/>
+      <c r="B24" s="21"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="21"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="20"/>
+      <c r="B25" s="21"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="21"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="20"/>
+      <c r="B26" s="21"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="21"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="20"/>
+      <c r="B27" s="21"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="21"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="20"/>
+      <c r="B28" s="21"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="21"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
+      <c r="B29" s="21"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="21"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="20"/>
+      <c r="B30" s="21"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="21"/>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="22"/>
+      <c r="B31" s="23"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="23"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
bibliographic work. comparing results started
</commit_message>
<xml_diff>
--- a/bibliografia/resumen_bibliografia.xlsx
+++ b/bibliografia/resumen_bibliografia.xlsx
@@ -5,19 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josee\Desktop\Departamento\formacion celulas\reproduccion_ulutas\bibliografia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\José Enrique\Desktop\cell-formation\cell-formation\bibliografia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCF7E3A-E32D-404A-B111-F7DE1A4EB681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742CBF93-4736-42B5-9DFB-2AF53EE094A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1080" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Articles" sheetId="1" r:id="rId1"/>
     <sheet name="Reviews" sheetId="2" r:id="rId2"/>
     <sheet name="ReviewKesavan2019" sheetId="3" r:id="rId3"/>
     <sheet name="ReviewPapaioannu2010" sheetId="5" r:id="rId4"/>
-    <sheet name="diccionario" sheetId="4" r:id="rId5"/>
+    <sheet name="ANN" sheetId="6" r:id="rId5"/>
+    <sheet name="diccionario" sheetId="4" r:id="rId6"/>
+    <sheet name="Revistas" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="213">
   <si>
     <t>Autor/res</t>
   </si>
@@ -103,122 +105,12 @@
     <t>El artículo más moderno que menciona es de 2013. Hace una separación temática que ni entiendo bien ni comparto.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">"The method presented in this paper has set a new benchmark GE for 5 of the 35 test instances used by the researchers in the context of machine-part cell formation without singletons." </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>FALSO, SOLO MEJORA 1 FRENTE A ULUTAS, A21</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(se compara con GA2)</t>
-    </r>
-  </si>
-  <si>
     <t>Rabbani</t>
   </si>
   <si>
     <t>Machine failure and workload balance</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Este trabajo me gusta (tiene 8 citas además. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>REVISAR BIBLIOGRAFÍA QUE LE CITA)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Non-dominated sorting</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> GA</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Multi-objective </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>particle</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>swarm</t>
-    </r>
-  </si>
-  <si>
     <t>Compara los dos algoritmos que presenta</t>
   </si>
   <si>
@@ -243,9 +135,6 @@
     <t>Nalluri</t>
   </si>
   <si>
-    <t>Tiene 10 citas</t>
-  </si>
-  <si>
     <t>Chaudhuri</t>
   </si>
   <si>
@@ -271,9 +160,6 @@
   </si>
   <si>
     <t>Srinivasan</t>
-  </si>
-  <si>
-    <t>ZODIAC: ideal seed algorithm for clustering</t>
   </si>
   <si>
     <t>GRAFICS: non-hierarchical clustering</t>
@@ -414,9 +300,6 @@
     <t>IPSO (particle swarm)</t>
   </si>
   <si>
-    <t>le añade inteligencia con una red neuronal (SOM)</t>
-  </si>
-  <si>
     <t>35 problemas, 30 mejoró</t>
   </si>
   <si>
@@ -474,9 +357,6 @@
     <t>MOSS with MADM</t>
   </si>
   <si>
-    <t>cell load and cost minimization</t>
-  </si>
-  <si>
     <t>SPEA-II and NSGA-I</t>
   </si>
   <si>
@@ -547,9 +427,6 @@
   </si>
   <si>
     <t>CSA</t>
-  </si>
-  <si>
-    <t>160+ citas</t>
   </si>
   <si>
     <t>Taxonomy and 
@@ -595,9 +472,6 @@
     <t xml:space="preserve">Similarity coefficient methods </t>
   </si>
   <si>
-    <t>2 Citas. Cita artículos algo más modernos. Se centra en heurísticas y meta-heurísticas de CFP y Cell-layout. Concluye que para enfrentar multiples problemas del CMS hace falta una hibridación metaheurística robusta. Multi-optimization da peores resultados individuales</t>
-  </si>
-  <si>
     <t>Mehdizadeh</t>
   </si>
   <si>
@@ -645,6 +519,205 @@
   </si>
   <si>
     <t>Multi-objective CFP</t>
+  </si>
+  <si>
+    <t>Utilization-based grouping efficacy</t>
+  </si>
+  <si>
+    <t>Dataset A y B (Bychkov).Obtiene los resultados mejores del benchmark para todos los problemas y da solución a problemas grandes (A35).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dice que mejora 5 de los problemas del dataset A pero solo se compara con artículos antiguos. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FALSO, SOLO MEJORA 1 FRENTE A ULUTAS (A21)</t>
+    </r>
+  </si>
+  <si>
+    <t>Multiobjective : cell load and cost minimization</t>
+  </si>
+  <si>
+    <t>Hopﬁeld neural network,</t>
+  </si>
+  <si>
+    <t>Chu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chattopadhyay et al. </t>
+  </si>
+  <si>
+    <t>Chen and Cheng</t>
+  </si>
+  <si>
+    <t>Guerrero et al.</t>
+  </si>
+  <si>
+    <t>Pandian and Mahapatra</t>
+  </si>
+  <si>
+    <t>Yang and Yang</t>
+  </si>
+  <si>
+    <t>adaptive resonance theory (ART), ART1 and so forth</t>
+  </si>
+  <si>
+    <t>backpropagation neural network</t>
+  </si>
+  <si>
+    <t>ANN</t>
+  </si>
+  <si>
+    <t>le añade inteligencia con una red neuronal (Self Organisation Map)</t>
+  </si>
+  <si>
+    <t>Noktehdan et al</t>
+  </si>
+  <si>
+    <t>eveloped a meta-heuristic algorithm to solve a class of grouping problems (bin packing, graph coloring, scheduling,</t>
+  </si>
+  <si>
+    <t>¡¡PRÁCTICAMENTE VIENE EL CÓDIGO!!
+Dataset A y otros 17 nuevos que no he visto.
+Mejora GE en el 27% de ellos</t>
+  </si>
+  <si>
+    <t>Bychkov and Batsyn</t>
+  </si>
+  <si>
+    <t>Pinheiro et al</t>
+  </si>
+  <si>
+    <t>An efﬁcient exact model for the cell formation problem with a variable number of production cells.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A matheuristic for the cell formation problem. </t>
+  </si>
+  <si>
+    <t>Zeb, Karoum, Bychkov, Mahmoodian, Pinheiro,Noktehdan</t>
+  </si>
+  <si>
+    <t>Elbenani</t>
+  </si>
+  <si>
+    <t>Genetic algorithm and large neighbourhood search to solve the cell formation problem</t>
+  </si>
+  <si>
+    <t>para enfrentar multiples problemas del CMS hace falta una hibridación metaheurística robusta. Multi-optimization da peores resultados individuales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Citas. Cita artículos algo más modernos. Se centra en heurísticas y meta-heurísticas de CFP y Cell-layout. </t>
+  </si>
+  <si>
+    <t>Objetivo del review</t>
+  </si>
+  <si>
+    <t>Conclusiones</t>
+  </si>
+  <si>
+    <t>160+ citas, pero es bastante antiguo.</t>
+  </si>
+  <si>
+    <t>Non-dominated sorting GA Multi-objective particle swarm</t>
+  </si>
+  <si>
+    <t>8 citas (REVISAR BIBLIOGRAFÍA QUE LE CITA)</t>
+  </si>
+  <si>
+    <t>Azadeh</t>
+  </si>
+  <si>
+    <t>Unique NSGA-II and MOPSO algorithms for improved dynamic cellular manufacturing systems considering human factors</t>
+  </si>
+  <si>
+    <t>Journal of Industrial Engineering International</t>
+  </si>
+  <si>
+    <t>European Journal of Industrial Engineering</t>
+  </si>
+  <si>
+    <t>1.18</t>
+  </si>
+  <si>
+    <t>JCI</t>
+  </si>
+  <si>
+    <t>COMPUTERS &amp; INDUSTRIAL ENGINEERING</t>
+  </si>
+  <si>
+    <t>Soft computing</t>
+  </si>
+  <si>
+    <t>0.87</t>
+  </si>
+  <si>
+    <t>Revista</t>
+  </si>
+  <si>
+    <t>Percentil Scopus</t>
+  </si>
+  <si>
+    <t>0.33</t>
+  </si>
+  <si>
+    <t>no residual cells allowed</t>
+  </si>
+  <si>
+    <t>dice Multiobjetivo (void+exceptions + intercel movements)
+al final usa GE</t>
+  </si>
+  <si>
+    <t>2 citas (una el mismo otra nalluri) en revista mala
+* Lévy flights (random selection)
+* local search Gonçalves 2004</t>
+  </si>
+  <si>
+    <t>An evolutionary algorithm for manufacturing cell formation</t>
+  </si>
+  <si>
+    <t>Gonçalves</t>
+  </si>
+  <si>
+    <t>Computer and Industrial Engineering</t>
+  </si>
+  <si>
+    <t>Creo que los resultados están falseados.</t>
+  </si>
+  <si>
+    <t>*CSA hibridizado con GA.  Tiene 10 citas en soft computing (REVISAR BIBLIOGRAFÍA QUE LE CITA)
+* New affinity function
+* New part assignment heuristic to map parts to machine cells
+* Machine cells -&gt; Part Families -&gt; Mapping
+* No dice nada de TIEMPO ni ITERACIONES</t>
+  </si>
+  <si>
+    <t>ZODIAC,GRAFICS,EA,SA,GRASP,GA-LNS</t>
+  </si>
+  <si>
+    <t>Cell formation using a simulated annealing algorithm with</t>
+  </si>
+  <si>
+    <t>variable neighbourhood</t>
+  </si>
+  <si>
+    <t>Ying, Lin, Lu</t>
+  </si>
+  <si>
+    <t>De los antiguos, según Karoum 2018, parece que eb este hay un salto de magnitud considerable</t>
+  </si>
+  <si>
+    <t>revisar el encoding de esta solución. De los antiguos, según Karoum 2018, parece que eb este hay un salto de magnitud considerable</t>
+  </si>
+  <si>
+    <t>Resultados equiparables a Elbenani2012 y Ying 2011</t>
   </si>
 </sst>
 </file>
@@ -814,7 +887,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -826,13 +899,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -877,12 +944,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -891,6 +952,39 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1172,10 +1266,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1183,40 +1277,41 @@
     <col min="1" max="1" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" style="3" customWidth="1"/>
     <col min="3" max="3" width="33" style="1" customWidth="1"/>
-    <col min="4" max="5" width="25.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" style="3" customWidth="1"/>
     <col min="6" max="6" width="32.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="51.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="77.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="87.5703125" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" s="8" t="s">
+      <c r="E1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H1" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1229,8 +1324,17 @@
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="F2" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1246,12 +1350,15 @@
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="3" t="s">
+      <c r="E3" s="8"/>
+      <c r="F3" s="25" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H3" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1268,208 +1375,323 @@
         <v>14</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="26">
         <v>2019</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5" t="s">
+      <c r="E5" s="26"/>
+      <c r="F5" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>49</v>
+      <c r="G5" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="29" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B6" s="3">
         <v>2020</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B7" s="3">
         <v>2020</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="24">
+        <v>2019</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="33"/>
+      <c r="F8" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="23" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="3">
+      <c r="B9" s="24">
         <v>2019</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B10" s="3">
         <v>2018</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B11" s="3">
         <v>2016</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
+        <v>46</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="27"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B12" s="3">
         <v>2016</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B13" s="3">
         <v>2016</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>154</v>
+        <v>147</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B14" s="3">
         <v>2021</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>161</v>
+        <v>148</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B15" s="3">
         <v>2021</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2016</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B17" s="3">
+        <v>2018</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>42</v>
+        <v>173</v>
       </c>
       <c r="B18" s="3">
+        <v>2017</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="B19" s="25">
+        <v>2012</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="E19" s="25"/>
+      <c r="H19" s="34" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B20" s="3">
+        <v>2017</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B21" s="3">
+        <v>2004</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="34" t="s">
+        <v>209</v>
+      </c>
+      <c r="B24" s="25">
+        <v>2011</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>207</v>
+      </c>
+      <c r="E24" s="25"/>
+      <c r="H24" s="35" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="3">
         <v>1987</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
+      <c r="C25" s="8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="3">
+        <v>1991</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1481,8 +1703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE49079E-D804-408A-9E73-9DA75E4351D1}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1491,88 +1713,83 @@
     <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24" customWidth="1"/>
-    <col min="8" max="8" width="71.85546875" style="15" customWidth="1"/>
+    <col min="5" max="6" width="27.5703125" customWidth="1"/>
+    <col min="7" max="7" width="53.42578125" customWidth="1"/>
+    <col min="8" max="8" width="71.85546875" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" s="8" t="s">
+      <c r="E1" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="26" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="G1" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="29" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="31">
         <v>2020</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24" t="s">
+      <c r="D2" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="26">
+        <v>2017</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="5">
-        <v>2017</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="D3" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3" s="29"/>
+      <c r="H3" s="29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B4" s="3">
         <v>2019</v>
@@ -1581,21 +1798,22 @@
         <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>19</v>
+        <v>51</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>179</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>146</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B5" s="3">
         <v>2020</v>
@@ -1604,71 +1822,65 @@
         <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="F5" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="10">
+        <v>2019</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="12">
-        <v>2019</v>
-      </c>
-      <c r="C6" s="11" t="s">
+      <c r="D6" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="24">
+        <v>2010</v>
+      </c>
+      <c r="C7" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="28">
-        <v>2010</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="27" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="D7" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B8" s="3">
         <v>2006</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F8" s="3"/>
+        <v>137</v>
+      </c>
+      <c r="F8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1680,7 +1892,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1697,307 +1909,307 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" s="8" t="s">
+      <c r="E1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>39</v>
+      <c r="H1" s="6" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B2" s="1">
         <v>2012</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B3" s="1">
         <v>2014</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B4" s="1">
         <v>2017</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>86</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B5" s="1">
         <v>2015</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G5" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B6" s="1">
         <v>2007</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B7" s="1">
         <v>2008</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="14">
+        <v>2010</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="H8" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" s="1" t="s">
+    </row>
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="B8" s="16">
-        <v>2010</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="B9" s="1">
         <v>2009</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>106</v>
+        <v>157</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B10" s="1">
         <v>2010</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B11" s="1">
         <v>2016</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B12" s="1">
         <v>2018</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B13" s="1">
         <v>2014</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B14" s="1">
         <v>2012</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>103</v>
+      <c r="C14" s="8" t="s">
+        <v>97</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>11</v>
@@ -2021,6 +2233,127 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D16B25-5325-47F3-A042-9F76F2F78785}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2">
+        <v>1997</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3">
+        <v>2012</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="I3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4">
+        <v>1995</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5">
+        <v>2002</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="I5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6">
+        <v>2009</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="I6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7">
+        <v>2008</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F67EBF-2A64-4E23-9654-8BB6149B5AE4}">
   <dimension ref="A1:E31"/>
   <sheetViews>
@@ -2035,252 +2368,318 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="19"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="19"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="E1" s="19" t="s">
+      <c r="D8" s="18"/>
+      <c r="E8" s="19"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="19"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="21"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="21"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="21"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="21"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="21"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="21"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="B10" s="21"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="21"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="21"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="19"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="21"/>
+      <c r="A12" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="19"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="21"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="21"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="19"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="19"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="21"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="21"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="19"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="19"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="21"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="21"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="19"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="19"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
-      <c r="B16" s="21"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="19"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="19"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="21"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="21"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="19"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="19"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="21"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="21"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="19"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="19"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="21"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="21"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="19"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="19"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="21"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="21"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="19"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="19"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
-      <c r="B21" s="21"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="21"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="19"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="19"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
-      <c r="B22" s="21"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="19"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="19"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
-      <c r="B23" s="21"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="21"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="19"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="19"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
-      <c r="B24" s="21"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="21"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="19"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="19"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
-      <c r="B25" s="21"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="21"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="19"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="19"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
-      <c r="B26" s="21"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="21"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="19"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="19"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
-      <c r="B27" s="21"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="21"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="19"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="19"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
-      <c r="B28" s="21"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="21"/>
+      <c r="A28" s="18"/>
+      <c r="B28" s="19"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="19"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
-      <c r="B29" s="21"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="21"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="19"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="19"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
-      <c r="B30" s="21"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="21"/>
+      <c r="A30" s="18"/>
+      <c r="B30" s="19"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="19"/>
     </row>
     <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="22"/>
-      <c r="B31" s="23"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="23"/>
+      <c r="A31" s="20"/>
+      <c r="B31" s="21"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CADD8E33-4657-4BD0-98A5-B60AA5D19BBF}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="12"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="12">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>197</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>